<commit_message>
Change the percentages to Ratios
</commit_message>
<xml_diff>
--- a/data/CO/2017-2018/2017-18 Student Teacher Ratios.xlsx
+++ b/data/CO/2017-2018/2017-18 Student Teacher Ratios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayush\Documents\GitHub\DS-5110-Group-Project\data\CO\2017-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF2A98AB-5702-40DE-B935-763C07EB5870}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7C42E81-E2F5-4B61-A0D2-E75127E159E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12363,7 +12363,7 @@
     <t>Teacher_FTE</t>
   </si>
   <si>
-    <t>Pupil/_Teacher_FTE_Ratio</t>
+    <t>Pupil_Teacher_FTE_Ratio</t>
   </si>
 </sst>
 </file>
@@ -12726,7 +12726,7 @@
   <dimension ref="A1:I1879"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>